<commit_message>
reportes & nuevos campos en estudiante
</commit_message>
<xml_diff>
--- a/src/report_details.xlsx
+++ b/src/report_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\next.js\SysProGestion\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14D30A2-3D78-4D53-B3E7-ADD7DFCD3E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051AED9D-034D-4CA0-AE1C-0E9638965649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>DETALLE DE PASANTES PERIODO 2023 - 2024</t>
   </si>
@@ -87,6 +87,21 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>VOTA?</t>
+  </si>
+  <si>
+    <t>CENTRO DE VOTACION</t>
+  </si>
+  <si>
+    <t>DEPENDENCIA</t>
+  </si>
+  <si>
+    <t>PARROQUIA DEL CENTRO DE VOTACIÓN</t>
+  </si>
+  <si>
+    <t>TELEFONO</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:S13"/>
+  <dimension ref="A6:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1072,16 +1087,18 @@
     <col min="16" max="16" width="13.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="15.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="19.85546875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="1"/>
+    <col min="19" max="19" width="30.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="34.140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:19" ht="51.75" customHeight="1">
+    <row r="6" spans="1:20" ht="51.75" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:19" s="13" customFormat="1" ht="30">
+    <row r="7" spans="1:20" s="13" customFormat="1" ht="30">
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
@@ -1109,38 +1126,41 @@
       <c r="I7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="L7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="N7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="O7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="Q7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20">
       <c r="H8" s="3"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1152,7 +1172,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:20">
       <c r="H9" s="3"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1164,7 +1184,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20">
       <c r="H10" s="3"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1176,7 +1196,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:20">
       <c r="H11" s="3"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1188,7 +1208,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20">
       <c r="H12" s="3"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1200,7 +1220,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20">
       <c r="H13" s="3"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>

</xml_diff>